<commit_message>
added qc_flag 4 for heated sample
</commit_message>
<xml_diff>
--- a/specific_variables/snow-temperature-profile.xlsx
+++ b/specific_variables/snow-temperature-profile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F86C02-A677-5F44-97C2-6CAAE11FD7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7431A5FB-4AE5-A743-8482-0B79F1C9572C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17240" yWindow="1860" windowWidth="20540" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,12 +88,6 @@
     <t>flag_meanings</t>
   </si>
   <si>
-    <t>0, 1, 2, 3</t>
-  </si>
-  <si>
-    <t>not_used good_data bad_data_temperature_outside_sensor_operational_range bad_data_unspecified_instrument_error</t>
-  </si>
-  <si>
     <t>temperature</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>0, 1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>not_used good_data bad_data_temperature_outside_sensor_operational_range bad_data_unspecified_instrument_error heated_sample</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
   <dimension ref="A1:C1013"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -620,7 +620,7 @@
     </row>
     <row r="2" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -640,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -658,7 +658,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -695,7 +695,7 @@
     </row>
     <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -728,7 +728,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -768,7 +768,7 @@
     </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -777,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -785,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -809,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -841,7 +841,7 @@
     </row>
     <row r="31" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" s="3"/>
     </row>
@@ -850,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -874,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -882,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -914,7 +914,7 @@
     </row>
     <row r="41" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C41" s="3"/>
     </row>
@@ -923,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -931,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,7 +947,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -955,7 +955,7 @@
         <v>10</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -987,7 +987,7 @@
     </row>
     <row r="51" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C51" s="3"/>
     </row>
@@ -1004,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1020,7 +1020,7 @@
         <v>9</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1028,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1060,7 +1060,7 @@
     </row>
     <row r="61" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
@@ -1098,7 +1098,7 @@
         <v>10</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1107,7 +1107,7 @@
         <v>20</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1116,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>